<commit_message>
polished up the tflite model
</commit_message>
<xml_diff>
--- a/Model Test/model5/dataCustom.xlsx
+++ b/Model Test/model5/dataCustom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Thushara Piyasekara\Downloads\IIT\Year 2 Semester 2\SDGP Implementaion\Diabuddies_SDGP\Model Test\model5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF42E0A0-7821-4EE8-ABBA-5C8FC97A2678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBB9AAD-1920-47FF-A833-7AD338979714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="84" yWindow="324" windowWidth="22956" windowHeight="12636" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,19 +49,19 @@
     <t>protein</t>
   </si>
   <si>
-    <t>Drinker</t>
+    <t>gender</t>
   </si>
   <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Age</t>
+    <t>age</t>
   </si>
   <si>
     <t>BMI</t>
   </si>
   <si>
     <t>Smoking</t>
+  </si>
+  <si>
+    <t>Drinker</t>
   </si>
   <si>
     <t>diabetes_duration</t>
@@ -468,22 +468,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.6640625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -514,19 +503,19 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>14</v>

</xml_diff>